<commit_message>
registro e ingreso funcionan al 90%
</commit_message>
<xml_diff>
--- a/static/data/products_complete.xlsx
+++ b/static/data/products_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8C08B1-94E3-43B5-B672-07BA94703CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0847DD4A-4ECA-4456-B812-71A7811C8DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="1053">
   <si>
     <t>product_slug</t>
   </si>
@@ -3111,7 +3111,85 @@
     <t>/media/product_images/invitaciones_papeleria/bodas/servilletas/servilletas.jpg</t>
   </si>
   <si>
-    <t>/media/product_images/invitaciones_papeleria/bodas/guarda_la_fecha/guarda_la_fecha.jpg</t>
+    <t>carteles-carton-espuma</t>
+  </si>
+  <si>
+    <t>Carteles de cartón espuma</t>
+  </si>
+  <si>
+    <t>CCE-001</t>
+  </si>
+  <si>
+    <t>Carteles para tu día especial</t>
+  </si>
+  <si>
+    <t>Invitaciones para tu boda</t>
+  </si>
+  <si>
+    <t>IB-001</t>
+  </si>
+  <si>
+    <t>Invitaciones elegantes para tu boda</t>
+  </si>
+  <si>
+    <t>Invitaciones para tu despedida de soltera</t>
+  </si>
+  <si>
+    <t>IDS-001</t>
+  </si>
+  <si>
+    <t>invitaciones-despedida-de-soltera</t>
+  </si>
+  <si>
+    <t>programa-de-boda</t>
+  </si>
+  <si>
+    <t>Programa de boda</t>
+  </si>
+  <si>
+    <t>PDB-001</t>
+  </si>
+  <si>
+    <t>libro-de-firmas</t>
+  </si>
+  <si>
+    <t>Libro de firmas de invitados</t>
+  </si>
+  <si>
+    <t>LDF-001</t>
+  </si>
+  <si>
+    <t>tarjetas-de-menu</t>
+  </si>
+  <si>
+    <t>Tarjetas de menú</t>
+  </si>
+  <si>
+    <t>TM-001</t>
+  </si>
+  <si>
+    <t>Tarjetas para el menú de la boda</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/carteles_carton_espuma/carteles-carton-espuma.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/invitaciones_despedida_de_soltera/invitaciones-despedida-de-soltera.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/programa_de_boda/programa-de-boda.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/libro_de_firmas/libro-de-firmas.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/tarjetas_de_menu/tarjetas-de-menu.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/guarda_la_fecha/guarda-la-fecha.jpg</t>
+  </si>
+  <si>
+    <t>/media/product_images/invitaciones_papeleria/bodas/invitaciones_de_boda/invitaciones-de-boda.jpg</t>
   </si>
 </sst>
 </file>
@@ -3958,16 +4036,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N166"/>
+  <dimension ref="A1:N172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+    <sheetView tabSelected="1" topLeftCell="B149" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="83.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -9109,7 +9188,7 @@
         <v>1023</v>
       </c>
       <c r="G165" t="s">
-        <v>1026</v>
+        <v>1051</v>
       </c>
       <c r="H165" t="s">
         <v>20</v>
@@ -9144,6 +9223,180 @@
         <v>20</v>
       </c>
       <c r="I166" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C167" t="s">
+        <v>344</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E167" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G167" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H167" t="s">
+        <v>20</v>
+      </c>
+      <c r="I167" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>345</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C168" t="s">
+        <v>344</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E168" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G168" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H168" t="s">
+        <v>20</v>
+      </c>
+      <c r="I168" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C169" t="s">
+        <v>344</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E169" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F169" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G169" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H169" t="s">
+        <v>20</v>
+      </c>
+      <c r="I169" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C170" t="s">
+        <v>344</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E170" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F170" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G170" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H170" t="s">
+        <v>20</v>
+      </c>
+      <c r="I170" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C171" t="s">
+        <v>344</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E171" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F171" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G171" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H171" t="s">
+        <v>20</v>
+      </c>
+      <c r="I171" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C172" t="s">
+        <v>344</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E172" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G172" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H172" t="s">
+        <v>20</v>
+      </c>
+      <c r="I172" t="s">
         <v>666</v>
       </c>
     </row>

</xml_diff>